<commit_message>
kati 8 dhe 9
</commit_message>
<xml_diff>
--- a/5-Njësit-Banesore/regjistri/Koordinatat.xlsx
+++ b/5-Njësit-Banesore/regjistri/Koordinatat.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="23">
   <si>
     <t>Nr</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Kati 7</t>
+  </si>
+  <si>
+    <t>Kati 8</t>
+  </si>
+  <si>
+    <t>Kati 9</t>
   </si>
 </sst>
 </file>
@@ -517,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J446"/>
+  <dimension ref="B2:J552"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A382" workbookViewId="0">
-      <selection activeCell="I396" sqref="I396"/>
+    <sheetView tabSelected="1" topLeftCell="A488" workbookViewId="0">
+      <selection activeCell="I502" sqref="I502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7486,7 +7492,7 @@
         <v>4693125.8782000002</v>
       </c>
       <c r="E396" s="5">
-        <v>643.82700000000011</v>
+        <v>646.77700000000004</v>
       </c>
       <c r="F396" s="4" t="s">
         <v>8</v>
@@ -7507,7 +7513,7 @@
         <v>4693129.7394999899</v>
       </c>
       <c r="E397" s="5">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F397" s="4" t="s">
         <v>8</v>
@@ -7525,7 +7531,7 @@
         <v>4693129.1098999903</v>
       </c>
       <c r="E398" s="5">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F398" s="4" t="s">
         <v>8</v>
@@ -7543,7 +7549,7 @@
         <v>4693134.1200999999</v>
       </c>
       <c r="E399" s="5">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F399" s="4" t="s">
         <v>8</v>
@@ -7561,7 +7567,7 @@
         <v>4693128.00589999</v>
       </c>
       <c r="E400" s="5">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F400" s="4" t="s">
         <v>8</v>
@@ -7579,7 +7585,7 @@
         <v>4693122.65059999</v>
       </c>
       <c r="E401" s="5">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F401" s="4" t="s">
         <v>8</v>
@@ -7597,7 +7603,7 @@
         <v>4693122.0210999902</v>
       </c>
       <c r="E402" s="5">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F402" s="4" t="s">
         <v>8</v>
@@ -7615,7 +7621,7 @@
         <v>4693118.3436999898</v>
       </c>
       <c r="E403" s="5">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F403" s="5" t="s">
         <v>8</v>
@@ -7633,7 +7639,7 @@
         <v>4693116.1777999904</v>
       </c>
       <c r="E404" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F404" s="5" t="s">
         <v>8</v>
@@ -7651,7 +7657,7 @@
         <v>4693119.02779999</v>
       </c>
       <c r="E405" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F405" s="5" t="s">
         <v>8</v>
@@ -7669,7 +7675,7 @@
         <v>4693119.1064999904</v>
       </c>
       <c r="E406" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F406" s="5" t="s">
         <v>8</v>
@@ -7687,7 +7693,7 @@
         <v>4693119.3362999996</v>
       </c>
       <c r="E407" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F407" s="5" t="s">
         <v>8</v>
@@ -7705,7 +7711,7 @@
         <v>4693119.4936999902</v>
       </c>
       <c r="E408" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F408" s="5" t="s">
         <v>8</v>
@@ -7723,7 +7729,7 @@
         <v>4693121.9483000003</v>
       </c>
       <c r="E409" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F409" s="5" t="s">
         <v>8</v>
@@ -7741,7 +7747,7 @@
         <v>4693121.79099999</v>
       </c>
       <c r="E410" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F410" s="5" t="s">
         <v>8</v>
@@ -7759,7 +7765,7 @@
         <v>4693125.6338</v>
       </c>
       <c r="E411" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F411" s="5" t="s">
         <v>8</v>
@@ -7777,7 +7783,7 @@
         <v>4693118.2567999903</v>
       </c>
       <c r="E412" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F412" s="5" t="s">
         <v>8</v>
@@ -7795,7 +7801,7 @@
         <v>4693113.1493999902</v>
       </c>
       <c r="E413" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F413" s="5" t="s">
         <v>8</v>
@@ -7813,7 +7819,7 @@
         <v>4693113.2949999897</v>
       </c>
       <c r="E414" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F414" s="5" t="s">
         <v>8</v>
@@ -7831,7 +7837,7 @@
         <v>4693108.9973999998</v>
       </c>
       <c r="E415" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F415" s="5" t="s">
         <v>8</v>
@@ -7849,7 +7855,7 @@
         <v>4693141.2703</v>
       </c>
       <c r="E416" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F416" s="5" t="s">
         <v>8</v>
@@ -7867,7 +7873,7 @@
         <v>4693134.7495999997</v>
       </c>
       <c r="E417" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F417" s="5" t="s">
         <v>8</v>
@@ -7885,7 +7891,7 @@
         <v>4693137.5078999903</v>
       </c>
       <c r="E418" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F418" s="5" t="s">
         <v>8</v>
@@ -7903,7 +7909,7 @@
         <v>4693137.3603999997</v>
       </c>
       <c r="E419" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F419" s="5" t="s">
         <v>8</v>
@@ -7921,7 +7927,7 @@
         <v>4693141.3587999903</v>
       </c>
       <c r="E420" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F420" s="5" t="s">
         <v>8</v>
@@ -7939,7 +7945,7 @@
         <v>4693144.2122</v>
       </c>
       <c r="E421" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F421" s="5" t="s">
         <v>8</v>
@@ -7957,7 +7963,7 @@
         <v>4693132.6124</v>
       </c>
       <c r="E422" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F422" s="5" t="s">
         <v>8</v>
@@ -7975,7 +7981,7 @@
         <v>4693132.4550000001</v>
       </c>
       <c r="E423" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F423" s="5" t="s">
         <v>8</v>
@@ -7993,7 +7999,7 @@
         <v>4693129.3291999903</v>
       </c>
       <c r="E424" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F424" s="5" t="s">
         <v>8</v>
@@ -8011,7 +8017,7 @@
         <v>4693129.9586999901</v>
       </c>
       <c r="E425" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F425" s="5" t="s">
         <v>8</v>
@@ -8029,7 +8035,7 @@
         <v>4693144.4420999903</v>
       </c>
       <c r="E426" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F426" s="5" t="s">
         <v>8</v>
@@ -8047,7 +8053,7 @@
         <v>4693144.7567999903</v>
       </c>
       <c r="E427" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F427" s="5" t="s">
         <v>8</v>
@@ -8065,7 +8071,7 @@
         <v>4693149.6756999902</v>
       </c>
       <c r="E428" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F428" s="5" t="s">
         <v>8</v>
@@ -8083,7 +8089,7 @@
         <v>4693149.5576999998</v>
       </c>
       <c r="E429" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F429" s="5" t="s">
         <v>8</v>
@@ -8101,7 +8107,7 @@
         <v>4693155.0734000001</v>
       </c>
       <c r="E430" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F430" s="5" t="s">
         <v>8</v>
@@ -8119,7 +8125,7 @@
         <v>4693147.6175999902</v>
       </c>
       <c r="E431" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F431" s="5" t="s">
         <v>8</v>
@@ -8137,7 +8143,7 @@
         <v>4693142.1019000001</v>
       </c>
       <c r="E432" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F432" s="5" t="s">
         <v>8</v>
@@ -8155,7 +8161,7 @@
         <v>4693141.9838999901</v>
       </c>
       <c r="E433" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F433" s="5" t="s">
         <v>8</v>
@@ -8173,7 +8179,7 @@
         <v>4693137.0649999902</v>
       </c>
       <c r="E434" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F434" s="5" t="s">
         <v>8</v>
@@ -8191,7 +8197,7 @@
         <v>4693137.3010999998</v>
       </c>
       <c r="E435" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F435" s="5" t="s">
         <v>8</v>
@@ -8209,7 +8215,7 @@
         <v>4693108.8870999897</v>
       </c>
       <c r="E436" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F436" s="5" t="s">
         <v>8</v>
@@ -8227,7 +8233,7 @@
         <v>4693108.6627999898</v>
       </c>
       <c r="E437" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F437" s="5" t="s">
         <v>8</v>
@@ -8245,7 +8251,7 @@
         <v>4693103.7438999899</v>
       </c>
       <c r="E438" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F438" s="5" t="s">
         <v>8</v>
@@ -8263,7 +8269,7 @@
         <v>4693103.8619999904</v>
       </c>
       <c r="E439" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F439" s="5" t="s">
         <v>8</v>
@@ -8281,7 +8287,7 @@
         <v>4693098.3461999996</v>
       </c>
       <c r="E440" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F440" s="5" t="s">
         <v>8</v>
@@ -8299,7 +8305,7 @@
         <v>4693105.8019999899</v>
       </c>
       <c r="E441" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F441" s="5" t="s">
         <v>8</v>
@@ -8317,7 +8323,7 @@
         <v>4693111.3176999995</v>
       </c>
       <c r="E442" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F442" s="5" t="s">
         <v>8</v>
@@ -8335,7 +8341,7 @@
         <v>4693111.43569999</v>
       </c>
       <c r="E443" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F443" s="5" t="s">
         <v>8</v>
@@ -8353,7 +8359,7 @@
         <v>4693116.4924999904</v>
       </c>
       <c r="E444" s="7">
-        <v>643.82700000000011</v>
+        <v>646.77700000000016</v>
       </c>
       <c r="F444" s="5" t="s">
         <v>8</v>
@@ -8395,13 +8401,1897 @@
         <v>12</v>
       </c>
       <c r="G446" s="11"/>
+    </row>
+    <row r="448" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B448" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C448" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D448" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E448" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F448" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G448" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="449" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B449" s="4">
+        <v>1</v>
+      </c>
+      <c r="C449" s="5">
+        <v>7511863.3491000002</v>
+      </c>
+      <c r="D449" s="5">
+        <v>4693125.8782000002</v>
+      </c>
+      <c r="E449" s="5">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F449" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G449" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I449" s="8"/>
+    </row>
+    <row r="450" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B450" s="4">
+        <v>2</v>
+      </c>
+      <c r="C450" s="5">
+        <v>7511865.0015000002</v>
+      </c>
+      <c r="D450" s="5">
+        <v>4693129.7394999899</v>
+      </c>
+      <c r="E450" s="5">
+        <v>649.72699999999998</v>
+      </c>
+      <c r="F450" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G450" s="10"/>
+    </row>
+    <row r="451" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B451" s="4">
+        <v>3</v>
+      </c>
+      <c r="C451" s="5">
+        <v>7511866.4725000001</v>
+      </c>
+      <c r="D451" s="5">
+        <v>4693129.1098999903</v>
+      </c>
+      <c r="E451" s="5">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F451" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G451" s="10"/>
+    </row>
+    <row r="452" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B452" s="4">
+        <v>4</v>
+      </c>
+      <c r="C452" s="5">
+        <v>7511868.6166000003</v>
+      </c>
+      <c r="D452" s="5">
+        <v>4693134.1200999999</v>
+      </c>
+      <c r="E452" s="5">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F452" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G452" s="10"/>
+    </row>
+    <row r="453" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B453" s="4">
+        <v>5</v>
+      </c>
+      <c r="C453" s="5">
+        <v>7511883.3492000001</v>
+      </c>
+      <c r="D453" s="5">
+        <v>4693128.00589999</v>
+      </c>
+      <c r="E453" s="5">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F453" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G453" s="10"/>
+    </row>
+    <row r="454" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B454" s="4">
+        <v>6</v>
+      </c>
+      <c r="C454" s="5">
+        <v>7511881.0574000003</v>
+      </c>
+      <c r="D454" s="5">
+        <v>4693122.65059999</v>
+      </c>
+      <c r="E454" s="5">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F454" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G454" s="10"/>
+    </row>
+    <row r="455" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B455" s="4">
+        <v>7</v>
+      </c>
+      <c r="C455" s="5">
+        <v>7511882.5284000002</v>
+      </c>
+      <c r="D455" s="5">
+        <v>4693122.0210999902</v>
+      </c>
+      <c r="E455" s="5">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F455" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G455" s="10"/>
+    </row>
+    <row r="456" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B456" s="4">
+        <v>8</v>
+      </c>
+      <c r="C456" s="5">
+        <v>7511880.9545999896</v>
+      </c>
+      <c r="D456" s="5">
+        <v>4693118.3436999898</v>
+      </c>
+      <c r="E456" s="5">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F456" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G456" s="10"/>
+    </row>
+    <row r="457" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B457" s="6">
+        <v>9</v>
+      </c>
+      <c r="C457" s="7">
+        <v>7511859.8503</v>
+      </c>
+      <c r="D457" s="7">
+        <v>4693116.1777999904</v>
+      </c>
+      <c r="E457" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F457" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G457" s="10"/>
+    </row>
+    <row r="458" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B458" s="6">
+        <v>10</v>
+      </c>
+      <c r="C458" s="7">
+        <v>7511861.0700000003</v>
+      </c>
+      <c r="D458" s="7">
+        <v>4693119.02779999</v>
+      </c>
+      <c r="E458" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F458" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G458" s="10"/>
+    </row>
+    <row r="459" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B459" s="6">
+        <v>11</v>
+      </c>
+      <c r="C459" s="7">
+        <v>7511860.8860999905</v>
+      </c>
+      <c r="D459" s="7">
+        <v>4693119.1064999904</v>
+      </c>
+      <c r="E459" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F459" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G459" s="10"/>
+    </row>
+    <row r="460" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B460" s="6">
+        <v>12</v>
+      </c>
+      <c r="C460" s="7">
+        <v>7511860.9845000003</v>
+      </c>
+      <c r="D460" s="7">
+        <v>4693119.3362999996</v>
+      </c>
+      <c r="E460" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F460" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G460" s="10"/>
+    </row>
+    <row r="461" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B461" s="6">
+        <v>13</v>
+      </c>
+      <c r="C461" s="7">
+        <v>7511860.6168</v>
+      </c>
+      <c r="D461" s="7">
+        <v>4693119.4936999902</v>
+      </c>
+      <c r="E461" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F461" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G461" s="10"/>
+    </row>
+    <row r="462" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B462" s="6">
+        <v>14</v>
+      </c>
+      <c r="C462" s="7">
+        <v>7511861.6672999896</v>
+      </c>
+      <c r="D462" s="7">
+        <v>4693121.9483000003</v>
+      </c>
+      <c r="E462" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F462" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G462" s="10"/>
+    </row>
+    <row r="463" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B463" s="6">
+        <v>15</v>
+      </c>
+      <c r="C463" s="7">
+        <v>7511862.0350000001</v>
+      </c>
+      <c r="D463" s="7">
+        <v>4693121.79099999</v>
+      </c>
+      <c r="E463" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F463" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G463" s="10"/>
+    </row>
+    <row r="464" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B464" s="6">
+        <v>16</v>
+      </c>
+      <c r="C464" s="7">
+        <v>7511863.6796000004</v>
+      </c>
+      <c r="D464" s="7">
+        <v>4693125.6338</v>
+      </c>
+      <c r="E464" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F464" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G464" s="10"/>
+    </row>
+    <row r="465" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B465" s="6">
+        <v>17</v>
+      </c>
+      <c r="C465" s="7">
+        <v>7511880.9173999904</v>
+      </c>
+      <c r="D465" s="7">
+        <v>4693118.2567999903</v>
+      </c>
+      <c r="E465" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F465" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G465" s="10"/>
+    </row>
+    <row r="466" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B466" s="6">
+        <v>18</v>
+      </c>
+      <c r="C466" s="7">
+        <v>7511878.7315999903</v>
+      </c>
+      <c r="D466" s="7">
+        <v>4693113.1493999902</v>
+      </c>
+      <c r="E466" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F466" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G466" s="10"/>
+    </row>
+    <row r="467" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B467" s="6">
+        <v>19</v>
+      </c>
+      <c r="C467" s="7">
+        <v>7511878.3914999897</v>
+      </c>
+      <c r="D467" s="7">
+        <v>4693113.2949999897</v>
+      </c>
+      <c r="E467" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F467" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G467" s="10"/>
+    </row>
+    <row r="468" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B468" s="6">
+        <v>20</v>
+      </c>
+      <c r="C468" s="7">
+        <v>7511876.5522999903</v>
+      </c>
+      <c r="D468" s="7">
+        <v>4693108.9973999998</v>
+      </c>
+      <c r="E468" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F468" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G468" s="10"/>
+    </row>
+    <row r="469" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B469" s="6">
+        <v>21</v>
+      </c>
+      <c r="C469" s="7">
+        <v>7511870.5888999896</v>
+      </c>
+      <c r="D469" s="7">
+        <v>4693141.2703</v>
+      </c>
+      <c r="E469" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F469" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G469" s="10"/>
+    </row>
+    <row r="470" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B470" s="6">
+        <v>22</v>
+      </c>
+      <c r="C470" s="7">
+        <v>7511867.1457000002</v>
+      </c>
+      <c r="D470" s="7">
+        <v>4693134.7495999997</v>
+      </c>
+      <c r="E470" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F470" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G470" s="10"/>
+    </row>
+    <row r="471" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B471" s="6">
+        <v>23</v>
+      </c>
+      <c r="C471" s="7">
+        <v>7511868.3261000002</v>
+      </c>
+      <c r="D471" s="7">
+        <v>4693137.5078999903</v>
+      </c>
+      <c r="E471" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F471" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G471" s="10"/>
+    </row>
+    <row r="472" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B472" s="6">
+        <v>24</v>
+      </c>
+      <c r="C472" s="7">
+        <v>7511868.6709000003</v>
+      </c>
+      <c r="D472" s="7">
+        <v>4693137.3603999997</v>
+      </c>
+      <c r="E472" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F472" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G472" s="10"/>
+    </row>
+    <row r="473" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B473" s="6">
+        <v>25</v>
+      </c>
+      <c r="C473" s="7">
+        <v>7511870.3821</v>
+      </c>
+      <c r="D473" s="7">
+        <v>4693141.3587999903</v>
+      </c>
+      <c r="E473" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F473" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G473" s="10"/>
+    </row>
+    <row r="474" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B474" s="6">
+        <v>26</v>
+      </c>
+      <c r="C474" s="7">
+        <v>7511871.8479000004</v>
+      </c>
+      <c r="D474" s="7">
+        <v>4693144.2122</v>
+      </c>
+      <c r="E474" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F474" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G474" s="10"/>
+    </row>
+    <row r="475" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B475" s="6">
+        <v>27</v>
+      </c>
+      <c r="C475" s="7">
+        <v>7511886.6259000003</v>
+      </c>
+      <c r="D475" s="7">
+        <v>4693132.6124</v>
+      </c>
+      <c r="E475" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F475" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G475" s="10"/>
+    </row>
+    <row r="476" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B476" s="6">
+        <v>28</v>
+      </c>
+      <c r="C476" s="7">
+        <v>7511886.9935999904</v>
+      </c>
+      <c r="D476" s="7">
+        <v>4693132.4550000001</v>
+      </c>
+      <c r="E476" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F476" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G476" s="10"/>
+    </row>
+    <row r="477" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B477" s="6">
+        <v>29</v>
+      </c>
+      <c r="C477" s="7">
+        <v>7511885.6558999904</v>
+      </c>
+      <c r="D477" s="7">
+        <v>4693129.3291999903</v>
+      </c>
+      <c r="E477" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F477" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G477" s="10"/>
+    </row>
+    <row r="478" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B478" s="6">
+        <v>30</v>
+      </c>
+      <c r="C478" s="7">
+        <v>7511884.1849999903</v>
+      </c>
+      <c r="D478" s="7">
+        <v>4693129.9586999901</v>
+      </c>
+      <c r="E478" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F478" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G478" s="10"/>
+    </row>
+    <row r="479" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B479" s="6">
+        <v>31</v>
+      </c>
+      <c r="C479" s="7">
+        <v>7511871.9463</v>
+      </c>
+      <c r="D479" s="7">
+        <v>4693144.4420999903</v>
+      </c>
+      <c r="E479" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F479" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G479" s="10"/>
+    </row>
+    <row r="480" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B480" s="6">
+        <v>32</v>
+      </c>
+      <c r="C480" s="7">
+        <v>7511871.2107999902</v>
+      </c>
+      <c r="D480" s="7">
+        <v>4693144.7567999903</v>
+      </c>
+      <c r="E480" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F480" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G480" s="10"/>
+    </row>
+    <row r="481" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B481" s="6">
+        <v>33</v>
+      </c>
+      <c r="C481" s="7">
+        <v>7511873.3158999896</v>
+      </c>
+      <c r="D481" s="7">
+        <v>4693149.6756999902</v>
+      </c>
+      <c r="E481" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F481" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G481" s="10"/>
+    </row>
+    <row r="482" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B482" s="6">
+        <v>34</v>
+      </c>
+      <c r="C482" s="7">
+        <v>7511873.5916999904</v>
+      </c>
+      <c r="D482" s="7">
+        <v>4693149.5576999998</v>
+      </c>
+      <c r="E482" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F482" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G482" s="10"/>
+    </row>
+    <row r="483" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B483" s="6">
+        <v>35</v>
+      </c>
+      <c r="C483" s="7">
+        <v>7511875.9522000002</v>
+      </c>
+      <c r="D483" s="7">
+        <v>4693155.0734000001</v>
+      </c>
+      <c r="E483" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F483" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G483" s="10"/>
+    </row>
+    <row r="484" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B484" s="6">
+        <v>36</v>
+      </c>
+      <c r="C484" s="7">
+        <v>7511893.3739</v>
+      </c>
+      <c r="D484" s="7">
+        <v>4693147.6175999902</v>
+      </c>
+      <c r="E484" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F484" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G484" s="10"/>
+    </row>
+    <row r="485" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B485" s="6">
+        <v>37</v>
+      </c>
+      <c r="C485" s="7">
+        <v>7511891.0133999903</v>
+      </c>
+      <c r="D485" s="7">
+        <v>4693142.1019000001</v>
+      </c>
+      <c r="E485" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F485" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G485" s="10"/>
+    </row>
+    <row r="486" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B486" s="6">
+        <v>38</v>
+      </c>
+      <c r="C486" s="7">
+        <v>7511891.2892000005</v>
+      </c>
+      <c r="D486" s="7">
+        <v>4693141.9838999901</v>
+      </c>
+      <c r="E486" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F486" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G486" s="10"/>
+    </row>
+    <row r="487" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B487" s="6">
+        <v>39</v>
+      </c>
+      <c r="C487" s="7">
+        <v>7511889.1841000002</v>
+      </c>
+      <c r="D487" s="7">
+        <v>4693137.0649999902</v>
+      </c>
+      <c r="E487" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F487" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G487" s="10"/>
+    </row>
+    <row r="488" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B488" s="6">
+        <v>40</v>
+      </c>
+      <c r="C488" s="7">
+        <v>7511888.6325000003</v>
+      </c>
+      <c r="D488" s="7">
+        <v>4693137.3010999998</v>
+      </c>
+      <c r="E488" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F488" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G488" s="10"/>
+    </row>
+    <row r="489" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B489" s="6">
+        <v>41</v>
+      </c>
+      <c r="C489" s="7">
+        <v>7511876.5050999904</v>
+      </c>
+      <c r="D489" s="7">
+        <v>4693108.8870999897</v>
+      </c>
+      <c r="E489" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F489" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G489" s="10"/>
+    </row>
+    <row r="490" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B490" s="6">
+        <v>42</v>
+      </c>
+      <c r="C490" s="7">
+        <v>7511877.0290999897</v>
+      </c>
+      <c r="D490" s="7">
+        <v>4693108.6627999898</v>
+      </c>
+      <c r="E490" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F490" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G490" s="10"/>
+    </row>
+    <row r="491" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B491" s="6">
+        <v>43</v>
+      </c>
+      <c r="C491" s="7">
+        <v>7511874.9239999903</v>
+      </c>
+      <c r="D491" s="7">
+        <v>4693103.7438999899</v>
+      </c>
+      <c r="E491" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F491" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G491" s="10"/>
+    </row>
+    <row r="492" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B492" s="6">
+        <v>44</v>
+      </c>
+      <c r="C492" s="7">
+        <v>7511874.6481999904</v>
+      </c>
+      <c r="D492" s="7">
+        <v>4693103.8619999904</v>
+      </c>
+      <c r="E492" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F492" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G492" s="10"/>
+    </row>
+    <row r="493" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B493" s="6">
+        <v>45</v>
+      </c>
+      <c r="C493" s="7">
+        <v>7511872.2877000002</v>
+      </c>
+      <c r="D493" s="7">
+        <v>4693098.3461999996</v>
+      </c>
+      <c r="E493" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F493" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G493" s="10"/>
+    </row>
+    <row r="494" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B494" s="6">
+        <v>46</v>
+      </c>
+      <c r="C494" s="7">
+        <v>7511854.8661000002</v>
+      </c>
+      <c r="D494" s="7">
+        <v>4693105.8019999899</v>
+      </c>
+      <c r="E494" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F494" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G494" s="10"/>
+    </row>
+    <row r="495" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B495" s="6">
+        <v>47</v>
+      </c>
+      <c r="C495" s="7">
+        <v>7511857.2265999904</v>
+      </c>
+      <c r="D495" s="7">
+        <v>4693111.3176999995</v>
+      </c>
+      <c r="E495" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F495" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G495" s="10"/>
+    </row>
+    <row r="496" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B496" s="6">
+        <v>48</v>
+      </c>
+      <c r="C496" s="7">
+        <v>7511856.9507999904</v>
+      </c>
+      <c r="D496" s="7">
+        <v>4693111.43569999</v>
+      </c>
+      <c r="E496" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F496" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G496" s="10"/>
+    </row>
+    <row r="497" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B497" s="6">
+        <v>49</v>
+      </c>
+      <c r="C497" s="7">
+        <v>7511859.1149000004</v>
+      </c>
+      <c r="D497" s="7">
+        <v>4693116.4924999904</v>
+      </c>
+      <c r="E497" s="7">
+        <v>649.72700000000009</v>
+      </c>
+      <c r="F497" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G497" s="10"/>
+    </row>
+    <row r="498" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B498" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C498" s="5">
+        <v>7511869.1087999996</v>
+      </c>
+      <c r="D498" s="5">
+        <v>4693143.5547000002</v>
+      </c>
+      <c r="E498" s="7">
+        <v>623.17700000000002</v>
+      </c>
+      <c r="F498" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G498" s="10"/>
+    </row>
+    <row r="499" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B499" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C499" s="5">
+        <v>7511858.3772</v>
+      </c>
+      <c r="D499" s="5">
+        <v>4693118.5031000003</v>
+      </c>
+      <c r="E499" s="7">
+        <v>623.17700000000002</v>
+      </c>
+      <c r="F499" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G499" s="11"/>
+    </row>
+    <row r="501" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B501" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C501" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D501" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E501" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F501" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G501" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="502" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B502" s="4">
+        <v>1</v>
+      </c>
+      <c r="C502" s="5">
+        <v>7511863.3491000002</v>
+      </c>
+      <c r="D502" s="5">
+        <v>4693125.8782000002</v>
+      </c>
+      <c r="E502" s="5">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F502" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G502" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I502" s="8"/>
+    </row>
+    <row r="503" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B503" s="4">
+        <v>2</v>
+      </c>
+      <c r="C503" s="5">
+        <v>7511865.0015000002</v>
+      </c>
+      <c r="D503" s="5">
+        <v>4693129.7394999899</v>
+      </c>
+      <c r="E503" s="5">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F503" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G503" s="10"/>
+    </row>
+    <row r="504" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B504" s="4">
+        <v>3</v>
+      </c>
+      <c r="C504" s="5">
+        <v>7511866.4725000001</v>
+      </c>
+      <c r="D504" s="5">
+        <v>4693129.1098999903</v>
+      </c>
+      <c r="E504" s="5">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F504" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G504" s="10"/>
+    </row>
+    <row r="505" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B505" s="4">
+        <v>4</v>
+      </c>
+      <c r="C505" s="5">
+        <v>7511868.6166000003</v>
+      </c>
+      <c r="D505" s="5">
+        <v>4693134.1200999999</v>
+      </c>
+      <c r="E505" s="5">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F505" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G505" s="10"/>
+    </row>
+    <row r="506" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B506" s="4">
+        <v>5</v>
+      </c>
+      <c r="C506" s="5">
+        <v>7511883.3492000001</v>
+      </c>
+      <c r="D506" s="5">
+        <v>4693128.00589999</v>
+      </c>
+      <c r="E506" s="5">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F506" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G506" s="10"/>
+    </row>
+    <row r="507" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B507" s="4">
+        <v>6</v>
+      </c>
+      <c r="C507" s="5">
+        <v>7511881.0574000003</v>
+      </c>
+      <c r="D507" s="5">
+        <v>4693122.65059999</v>
+      </c>
+      <c r="E507" s="5">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F507" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G507" s="10"/>
+    </row>
+    <row r="508" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B508" s="4">
+        <v>7</v>
+      </c>
+      <c r="C508" s="5">
+        <v>7511882.5284000002</v>
+      </c>
+      <c r="D508" s="5">
+        <v>4693122.0210999902</v>
+      </c>
+      <c r="E508" s="5">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F508" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G508" s="10"/>
+    </row>
+    <row r="509" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B509" s="4">
+        <v>8</v>
+      </c>
+      <c r="C509" s="5">
+        <v>7511880.9545999896</v>
+      </c>
+      <c r="D509" s="5">
+        <v>4693118.3436999898</v>
+      </c>
+      <c r="E509" s="5">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F509" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G509" s="10"/>
+    </row>
+    <row r="510" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B510" s="6">
+        <v>9</v>
+      </c>
+      <c r="C510" s="7">
+        <v>7511859.8503</v>
+      </c>
+      <c r="D510" s="7">
+        <v>4693116.1777999904</v>
+      </c>
+      <c r="E510" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F510" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G510" s="10"/>
+    </row>
+    <row r="511" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B511" s="6">
+        <v>10</v>
+      </c>
+      <c r="C511" s="7">
+        <v>7511861.0700000003</v>
+      </c>
+      <c r="D511" s="7">
+        <v>4693119.02779999</v>
+      </c>
+      <c r="E511" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F511" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G511" s="10"/>
+    </row>
+    <row r="512" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B512" s="6">
+        <v>11</v>
+      </c>
+      <c r="C512" s="7">
+        <v>7511860.8860999905</v>
+      </c>
+      <c r="D512" s="7">
+        <v>4693119.1064999904</v>
+      </c>
+      <c r="E512" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F512" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G512" s="10"/>
+    </row>
+    <row r="513" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B513" s="6">
+        <v>12</v>
+      </c>
+      <c r="C513" s="7">
+        <v>7511860.9845000003</v>
+      </c>
+      <c r="D513" s="7">
+        <v>4693119.3362999996</v>
+      </c>
+      <c r="E513" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F513" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G513" s="10"/>
+    </row>
+    <row r="514" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B514" s="6">
+        <v>13</v>
+      </c>
+      <c r="C514" s="7">
+        <v>7511860.6168</v>
+      </c>
+      <c r="D514" s="7">
+        <v>4693119.4936999902</v>
+      </c>
+      <c r="E514" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F514" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G514" s="10"/>
+    </row>
+    <row r="515" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B515" s="6">
+        <v>14</v>
+      </c>
+      <c r="C515" s="7">
+        <v>7511861.6672999896</v>
+      </c>
+      <c r="D515" s="7">
+        <v>4693121.9483000003</v>
+      </c>
+      <c r="E515" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F515" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G515" s="10"/>
+    </row>
+    <row r="516" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B516" s="6">
+        <v>15</v>
+      </c>
+      <c r="C516" s="7">
+        <v>7511862.0350000001</v>
+      </c>
+      <c r="D516" s="7">
+        <v>4693121.79099999</v>
+      </c>
+      <c r="E516" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F516" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G516" s="10"/>
+    </row>
+    <row r="517" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B517" s="6">
+        <v>16</v>
+      </c>
+      <c r="C517" s="7">
+        <v>7511863.6796000004</v>
+      </c>
+      <c r="D517" s="7">
+        <v>4693125.6338</v>
+      </c>
+      <c r="E517" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F517" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G517" s="10"/>
+    </row>
+    <row r="518" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B518" s="6">
+        <v>17</v>
+      </c>
+      <c r="C518" s="7">
+        <v>7511880.9173999904</v>
+      </c>
+      <c r="D518" s="7">
+        <v>4693118.2567999903</v>
+      </c>
+      <c r="E518" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F518" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G518" s="10"/>
+    </row>
+    <row r="519" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B519" s="6">
+        <v>18</v>
+      </c>
+      <c r="C519" s="7">
+        <v>7511878.7315999903</v>
+      </c>
+      <c r="D519" s="7">
+        <v>4693113.1493999902</v>
+      </c>
+      <c r="E519" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F519" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G519" s="10"/>
+    </row>
+    <row r="520" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B520" s="6">
+        <v>19</v>
+      </c>
+      <c r="C520" s="7">
+        <v>7511878.3914999897</v>
+      </c>
+      <c r="D520" s="7">
+        <v>4693113.2949999897</v>
+      </c>
+      <c r="E520" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F520" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G520" s="10"/>
+    </row>
+    <row r="521" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B521" s="6">
+        <v>20</v>
+      </c>
+      <c r="C521" s="7">
+        <v>7511876.5522999903</v>
+      </c>
+      <c r="D521" s="7">
+        <v>4693108.9973999998</v>
+      </c>
+      <c r="E521" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F521" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G521" s="10"/>
+    </row>
+    <row r="522" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B522" s="6">
+        <v>21</v>
+      </c>
+      <c r="C522" s="7">
+        <v>7511870.5888999896</v>
+      </c>
+      <c r="D522" s="7">
+        <v>4693141.2703</v>
+      </c>
+      <c r="E522" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F522" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G522" s="10"/>
+    </row>
+    <row r="523" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B523" s="6">
+        <v>22</v>
+      </c>
+      <c r="C523" s="7">
+        <v>7511867.1457000002</v>
+      </c>
+      <c r="D523" s="7">
+        <v>4693134.7495999997</v>
+      </c>
+      <c r="E523" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F523" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G523" s="10"/>
+    </row>
+    <row r="524" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B524" s="6">
+        <v>23</v>
+      </c>
+      <c r="C524" s="7">
+        <v>7511868.3261000002</v>
+      </c>
+      <c r="D524" s="7">
+        <v>4693137.5078999903</v>
+      </c>
+      <c r="E524" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F524" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G524" s="10"/>
+    </row>
+    <row r="525" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B525" s="6">
+        <v>24</v>
+      </c>
+      <c r="C525" s="7">
+        <v>7511868.6709000003</v>
+      </c>
+      <c r="D525" s="7">
+        <v>4693137.3603999997</v>
+      </c>
+      <c r="E525" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F525" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G525" s="10"/>
+    </row>
+    <row r="526" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B526" s="6">
+        <v>25</v>
+      </c>
+      <c r="C526" s="7">
+        <v>7511870.3821</v>
+      </c>
+      <c r="D526" s="7">
+        <v>4693141.3587999903</v>
+      </c>
+      <c r="E526" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F526" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G526" s="10"/>
+    </row>
+    <row r="527" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B527" s="6">
+        <v>26</v>
+      </c>
+      <c r="C527" s="7">
+        <v>7511871.8479000004</v>
+      </c>
+      <c r="D527" s="7">
+        <v>4693144.2122</v>
+      </c>
+      <c r="E527" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F527" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G527" s="10"/>
+    </row>
+    <row r="528" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B528" s="6">
+        <v>27</v>
+      </c>
+      <c r="C528" s="7">
+        <v>7511886.6259000003</v>
+      </c>
+      <c r="D528" s="7">
+        <v>4693132.6124</v>
+      </c>
+      <c r="E528" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F528" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G528" s="10"/>
+    </row>
+    <row r="529" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B529" s="6">
+        <v>28</v>
+      </c>
+      <c r="C529" s="7">
+        <v>7511886.9935999904</v>
+      </c>
+      <c r="D529" s="7">
+        <v>4693132.4550000001</v>
+      </c>
+      <c r="E529" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F529" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G529" s="10"/>
+    </row>
+    <row r="530" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B530" s="6">
+        <v>29</v>
+      </c>
+      <c r="C530" s="7">
+        <v>7511885.6558999904</v>
+      </c>
+      <c r="D530" s="7">
+        <v>4693129.3291999903</v>
+      </c>
+      <c r="E530" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F530" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G530" s="10"/>
+    </row>
+    <row r="531" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B531" s="6">
+        <v>30</v>
+      </c>
+      <c r="C531" s="7">
+        <v>7511884.1849999903</v>
+      </c>
+      <c r="D531" s="7">
+        <v>4693129.9586999901</v>
+      </c>
+      <c r="E531" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F531" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G531" s="10"/>
+    </row>
+    <row r="532" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B532" s="6">
+        <v>31</v>
+      </c>
+      <c r="C532" s="7">
+        <v>7511871.9463</v>
+      </c>
+      <c r="D532" s="7">
+        <v>4693144.4420999903</v>
+      </c>
+      <c r="E532" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F532" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G532" s="10"/>
+    </row>
+    <row r="533" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B533" s="6">
+        <v>32</v>
+      </c>
+      <c r="C533" s="7">
+        <v>7511871.2107999902</v>
+      </c>
+      <c r="D533" s="7">
+        <v>4693144.7567999903</v>
+      </c>
+      <c r="E533" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F533" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G533" s="10"/>
+    </row>
+    <row r="534" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B534" s="6">
+        <v>33</v>
+      </c>
+      <c r="C534" s="7">
+        <v>7511873.3158999896</v>
+      </c>
+      <c r="D534" s="7">
+        <v>4693149.6756999902</v>
+      </c>
+      <c r="E534" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F534" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G534" s="10"/>
+    </row>
+    <row r="535" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B535" s="6">
+        <v>34</v>
+      </c>
+      <c r="C535" s="7">
+        <v>7511873.5916999904</v>
+      </c>
+      <c r="D535" s="7">
+        <v>4693149.5576999998</v>
+      </c>
+      <c r="E535" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F535" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G535" s="10"/>
+    </row>
+    <row r="536" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B536" s="6">
+        <v>35</v>
+      </c>
+      <c r="C536" s="7">
+        <v>7511875.9522000002</v>
+      </c>
+      <c r="D536" s="7">
+        <v>4693155.0734000001</v>
+      </c>
+      <c r="E536" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F536" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G536" s="10"/>
+    </row>
+    <row r="537" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B537" s="6">
+        <v>36</v>
+      </c>
+      <c r="C537" s="7">
+        <v>7511893.3739</v>
+      </c>
+      <c r="D537" s="7">
+        <v>4693147.6175999902</v>
+      </c>
+      <c r="E537" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F537" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G537" s="10"/>
+    </row>
+    <row r="538" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B538" s="6">
+        <v>37</v>
+      </c>
+      <c r="C538" s="7">
+        <v>7511891.0133999903</v>
+      </c>
+      <c r="D538" s="7">
+        <v>4693142.1019000001</v>
+      </c>
+      <c r="E538" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F538" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G538" s="10"/>
+    </row>
+    <row r="539" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B539" s="6">
+        <v>38</v>
+      </c>
+      <c r="C539" s="7">
+        <v>7511891.2892000005</v>
+      </c>
+      <c r="D539" s="7">
+        <v>4693141.9838999901</v>
+      </c>
+      <c r="E539" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F539" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G539" s="10"/>
+    </row>
+    <row r="540" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B540" s="6">
+        <v>39</v>
+      </c>
+      <c r="C540" s="7">
+        <v>7511889.1841000002</v>
+      </c>
+      <c r="D540" s="7">
+        <v>4693137.0649999902</v>
+      </c>
+      <c r="E540" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F540" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G540" s="10"/>
+    </row>
+    <row r="541" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B541" s="6">
+        <v>40</v>
+      </c>
+      <c r="C541" s="7">
+        <v>7511888.6325000003</v>
+      </c>
+      <c r="D541" s="7">
+        <v>4693137.3010999998</v>
+      </c>
+      <c r="E541" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F541" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G541" s="10"/>
+    </row>
+    <row r="542" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B542" s="6">
+        <v>41</v>
+      </c>
+      <c r="C542" s="7">
+        <v>7511876.5050999904</v>
+      </c>
+      <c r="D542" s="7">
+        <v>4693108.8870999897</v>
+      </c>
+      <c r="E542" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F542" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G542" s="10"/>
+    </row>
+    <row r="543" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B543" s="6">
+        <v>42</v>
+      </c>
+      <c r="C543" s="7">
+        <v>7511877.0290999897</v>
+      </c>
+      <c r="D543" s="7">
+        <v>4693108.6627999898</v>
+      </c>
+      <c r="E543" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F543" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G543" s="10"/>
+    </row>
+    <row r="544" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B544" s="6">
+        <v>43</v>
+      </c>
+      <c r="C544" s="7">
+        <v>7511874.9239999903</v>
+      </c>
+      <c r="D544" s="7">
+        <v>4693103.7438999899</v>
+      </c>
+      <c r="E544" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F544" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G544" s="10"/>
+    </row>
+    <row r="545" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B545" s="6">
+        <v>44</v>
+      </c>
+      <c r="C545" s="7">
+        <v>7511874.6481999904</v>
+      </c>
+      <c r="D545" s="7">
+        <v>4693103.8619999904</v>
+      </c>
+      <c r="E545" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F545" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G545" s="10"/>
+    </row>
+    <row r="546" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B546" s="6">
+        <v>45</v>
+      </c>
+      <c r="C546" s="7">
+        <v>7511872.2877000002</v>
+      </c>
+      <c r="D546" s="7">
+        <v>4693098.3461999996</v>
+      </c>
+      <c r="E546" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F546" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G546" s="10"/>
+    </row>
+    <row r="547" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B547" s="6">
+        <v>46</v>
+      </c>
+      <c r="C547" s="7">
+        <v>7511854.8661000002</v>
+      </c>
+      <c r="D547" s="7">
+        <v>4693105.8019999899</v>
+      </c>
+      <c r="E547" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F547" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G547" s="10"/>
+    </row>
+    <row r="548" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B548" s="6">
+        <v>47</v>
+      </c>
+      <c r="C548" s="7">
+        <v>7511857.2265999904</v>
+      </c>
+      <c r="D548" s="7">
+        <v>4693111.3176999995</v>
+      </c>
+      <c r="E548" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F548" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G548" s="10"/>
+    </row>
+    <row r="549" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B549" s="6">
+        <v>48</v>
+      </c>
+      <c r="C549" s="7">
+        <v>7511856.9507999904</v>
+      </c>
+      <c r="D549" s="7">
+        <v>4693111.43569999</v>
+      </c>
+      <c r="E549" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F549" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G549" s="10"/>
+    </row>
+    <row r="550" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B550" s="6">
+        <v>49</v>
+      </c>
+      <c r="C550" s="7">
+        <v>7511859.1149000004</v>
+      </c>
+      <c r="D550" s="7">
+        <v>4693116.4924999904</v>
+      </c>
+      <c r="E550" s="7">
+        <v>652.67700000000013</v>
+      </c>
+      <c r="F550" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G550" s="10"/>
+    </row>
+    <row r="551" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B551" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C551" s="5">
+        <v>7511869.1087999996</v>
+      </c>
+      <c r="D551" s="5">
+        <v>4693143.5547000002</v>
+      </c>
+      <c r="E551" s="7">
+        <v>623.17700000000002</v>
+      </c>
+      <c r="F551" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G551" s="10"/>
+    </row>
+    <row r="552" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B552" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C552" s="5">
+        <v>7511858.3772</v>
+      </c>
+      <c r="D552" s="5">
+        <v>4693118.5031000003</v>
+      </c>
+      <c r="E552" s="7">
+        <v>623.17700000000002</v>
+      </c>
+      <c r="F552" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G552" s="11"/>
     </row>
   </sheetData>
   <sortState ref="B1:D21">
     <sortCondition ref="B1"/>
   </sortState>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="G396:G446"/>
+    <mergeCell ref="G449:G499"/>
+    <mergeCell ref="G502:G552"/>
     <mergeCell ref="E3:E10"/>
     <mergeCell ref="G13:G20"/>
     <mergeCell ref="G23:G73"/>

</xml_diff>

<commit_message>
te dhenat ne shape
</commit_message>
<xml_diff>
--- a/5-Njësit-Banesore/regjistri/Koordinatat.xlsx
+++ b/5-Njësit-Banesore/regjistri/Koordinatat.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J552"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A488" workbookViewId="0">
-      <selection activeCell="I502" sqref="I502"/>
+    <sheetView tabSelected="1" topLeftCell="A494" workbookViewId="0">
+      <selection activeCell="I503" sqref="I503"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9395,7 +9395,7 @@
         <v>4693129.7394999899</v>
       </c>
       <c r="E503" s="5">
-        <v>652.67700000000013</v>
+        <v>652.67700000000002</v>
       </c>
       <c r="F503" s="4" t="s">
         <v>8</v>

</xml_diff>